<commit_message>
Using formulas and functions -updated scoreboard
</commit_message>
<xml_diff>
--- a/Modifying the worksheet.xlsx
+++ b/Modifying the worksheet.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49402A55-6B7E-43A0-9A9D-4BA36360791D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9F142B-B2EB-48A1-9534-B65DAAEC535C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="4" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Dataset" sheetId="4" r:id="rId1"/>
     <sheet name="Sales Data" sheetId="1" r:id="rId2"/>
     <sheet name="Financial Data" sheetId="2" r:id="rId3"/>
-    <sheet name="Financial Scorecard" sheetId="3" r:id="rId4"/>
-    <sheet name="Sales Report 2018 2019" sheetId="6" r:id="rId5"/>
+    <sheet name="Sales Report 2018 2019" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -563,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,6 +572,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -636,9 +641,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,10 +652,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -974,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,10 +1095,6 @@
       <c r="P2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q2">
-        <f>AVERAGE(J2:J20)</f>
-        <v>276986.5263157895</v>
-      </c>
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1134,10 +1137,6 @@
       <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3">
-        <f>MAX(J2:J20)</f>
-        <v>461214</v>
-      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1178,10 +1177,6 @@
       </c>
       <c r="P4" t="s">
         <v>33</v>
-      </c>
-      <c r="Q4">
-        <f>MIN(J2:J20)</f>
-        <v>125319</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1835,7 +1830,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,11 +2483,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2634,7 @@
         <v>83606</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="0"/>
+        <f>D5-E5</f>
         <v>149649</v>
       </c>
       <c r="G5" s="2">
@@ -3072,74 +3067,54 @@
         <v>56453</v>
       </c>
     </row>
+    <row r="24" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="19">
+        <f>AVERAGE(D2:D20)</f>
+        <v>276986.5263157895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="19">
+        <f>MAX(D2:D20)</f>
+        <v>461214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="19">
+        <f>MIN(D2:D20)</f>
+        <v>125319</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E24:F24"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F40AB-1F15-4573-AC0C-90024DE33C6E}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2">
-        <v>276986.5263157895</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2">
-        <v>461214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2">
-        <v>125319</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EDE02B-1AE3-472A-9AA4-105EF5FD6642}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3150,19 +3125,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3170,64 +3145,64 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D4" s="14">
+      <c r="D4" s="17">
         <v>2018</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17">
         <v>2019</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3241,28 +3216,28 @@
       <c r="C6" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>294470</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <v>186951</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <v>367618</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <v>231313</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <v>104650</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <v>194875</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="16">
         <v>213221</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="16">
         <v>193992</v>
       </c>
     </row>
@@ -3276,28 +3251,28 @@
       <c r="C7" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>242379</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>165761</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <v>242191</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <v>248558</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>150298</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <v>250131</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <v>262538</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="16">
         <v>195802</v>
       </c>
     </row>
@@ -3311,28 +3286,28 @@
       <c r="C8" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>280973</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <v>354725</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <v>100058</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <v>159938</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <v>413803</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <v>367772</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="16">
         <v>284116</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="16">
         <v>321618</v>
       </c>
     </row>
@@ -3346,16 +3321,16 @@
       <c r="C9" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16">
         <v>123453</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="16">
         <v>287457</v>
       </c>
     </row>
@@ -3369,28 +3344,28 @@
       <c r="C10" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>97664</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>175113</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <v>145525</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="16">
         <v>115866</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="16">
         <v>231794</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <v>214229</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="16">
         <v>302197</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="16">
         <v>360759</v>
       </c>
     </row>
@@ -3404,24 +3379,24 @@
       <c r="C11" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16">
         <v>95423</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="16">
         <v>127835</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="16">
         <v>406324</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <v>423569</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="16">
         <v>160758</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="16">
         <v>287874</v>
       </c>
     </row>
@@ -3435,28 +3410,28 @@
       <c r="C12" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>96072</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <v>322071</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <v>337517</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <v>146034</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="16">
         <v>364865</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="16">
         <v>414727</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="16">
         <v>250822</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="16">
         <v>423552</v>
       </c>
     </row>
@@ -3470,28 +3445,28 @@
       <c r="C13" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>261518</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <v>183920</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="16">
         <v>202946</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="16">
         <v>205904</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="16">
         <v>224682</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="16">
         <v>276694</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="16">
         <v>261209</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="16">
         <v>348653</v>
       </c>
     </row>
@@ -3505,14 +3480,14 @@
       <c r="C14" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16">
         <v>241172</v>
       </c>
     </row>
@@ -3526,28 +3501,28 @@
       <c r="C15" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>212265</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <v>208190</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="16">
         <v>210727</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="16">
         <v>93406</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="16">
         <v>233555</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="16">
         <v>121487</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="16">
         <v>350045</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="16">
         <v>145471</v>
       </c>
     </row>
@@ -3561,28 +3536,28 @@
       <c r="C16" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="16">
         <v>104533</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="16">
         <v>331448</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="16">
         <v>197325</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="16">
         <v>207426</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="16">
         <v>267857</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="16">
         <v>220092</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="16">
         <v>114437</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="16">
         <v>119241</v>
       </c>
     </row>
@@ -3596,28 +3571,28 @@
       <c r="C17" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>324209</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>253397</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="16">
         <v>298893</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="16">
         <v>116472</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="16">
         <v>209008</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="16">
         <v>284024</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="16">
         <v>295343</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="16">
         <v>303757</v>
       </c>
     </row>
@@ -3631,28 +3606,28 @@
       <c r="C18" t="s">
         <v>144</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <v>182673</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <v>338317</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="16">
         <v>224638</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="16">
         <v>199913</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="16">
         <v>157338</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="16">
         <v>438173</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="16">
         <v>416473</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="16">
         <v>242891</v>
       </c>
     </row>
@@ -3666,28 +3641,28 @@
       <c r="C19" t="s">
         <v>145</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>359697</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <v>395046</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="16">
         <v>129871</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="16">
         <v>112396</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="16">
         <v>185351</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="16">
         <v>172879</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="16">
         <v>415627</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="16">
         <v>224008</v>
       </c>
     </row>
@@ -3701,18 +3676,18 @@
       <c r="C20" t="s">
         <v>146</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16">
         <v>101622</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="16">
         <v>120465</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="16">
         <v>262537</v>
       </c>
     </row>
@@ -3726,28 +3701,28 @@
       <c r="C21" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="16">
         <v>281335</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="16">
         <v>290674</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <v>213416</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="16">
         <v>138896</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="16">
         <v>148716</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="16">
         <v>440788</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="16">
         <v>118717</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="16">
         <v>295393</v>
       </c>
     </row>
@@ -3761,28 +3736,28 @@
       <c r="C22" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <v>393053</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="16">
         <v>155131</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <v>197972</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="16">
         <v>347987</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="16">
         <v>120062</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="16">
         <v>402641</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="16">
         <v>426099</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="16">
         <v>442987</v>
       </c>
     </row>
@@ -3796,28 +3771,28 @@
       <c r="C23" t="s">
         <v>149</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="16">
         <v>119379</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="16">
         <v>160105</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <v>219178</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="16">
         <v>189883</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="16">
         <v>146168</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="16">
         <v>237376</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="16">
         <v>344725</v>
       </c>
-      <c r="K23" s="18">
+      <c r="K23" s="16">
         <v>243717</v>
       </c>
     </row>
@@ -3831,26 +3806,26 @@
       <c r="C24" t="s">
         <v>150</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16">
         <v>101900</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="16">
         <v>364528</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="16">
         <v>211122</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="16">
         <v>354140</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="16">
         <v>193108</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="16">
         <v>248584</v>
       </c>
-      <c r="K24" s="18">
+      <c r="K24" s="16">
         <v>233292</v>
       </c>
     </row>
@@ -3864,28 +3839,28 @@
       <c r="C25" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="16">
         <v>128355</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="16">
         <v>135572</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <v>173208</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="16">
         <v>264144</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="16">
         <v>438135</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="16">
         <v>303683</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="16">
         <v>446278</v>
       </c>
-      <c r="K25" s="18">
+      <c r="K25" s="16">
         <v>262490</v>
       </c>
     </row>
@@ -3899,14 +3874,14 @@
       <c r="C26" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="16">
         <v>289224</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="16">
         <v>194600</v>
       </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -3918,35 +3893,35 @@
       <c r="C27" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="16">
         <f>SUMIF($B$6:$B$26,$B27,D$6:D$26)</f>
         <v>961526</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="16">
         <f t="shared" ref="E27:K27" si="0">SUMIF($B$6:$B$26,$B27,E$6:E$26)</f>
         <v>965665</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="16">
         <f t="shared" si="0"/>
         <v>976449</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="16">
         <f t="shared" si="0"/>
         <v>658349</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="16">
         <f t="shared" si="0"/>
         <v>750199</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="16">
         <f t="shared" si="0"/>
         <v>1093815</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="16">
         <f t="shared" si="0"/>
         <v>1324399</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="16">
         <f t="shared" si="0"/>
         <v>887921</v>
       </c>
@@ -3961,35 +3936,35 @@
       <c r="C28" t="s">
         <v>157</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="16">
         <f t="shared" ref="D28:K31" si="1">SUMIF($B$6:$B$26,$B28,D$6:D$26)</f>
         <v>802381</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="16">
         <f t="shared" si="1"/>
         <v>645428</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="16">
         <f t="shared" si="1"/>
         <v>471238</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="16">
         <f t="shared" si="1"/>
         <v>772069</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="16">
         <f t="shared" si="1"/>
         <v>972000</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="16">
         <f t="shared" si="1"/>
         <v>1074096</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="16">
         <f t="shared" si="1"/>
         <v>1156493</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="16">
         <f t="shared" si="1"/>
         <v>1027095</v>
       </c>
@@ -4004,35 +3979,35 @@
       <c r="C29" t="s">
         <v>157</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="16">
         <f t="shared" si="1"/>
         <v>261518</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="16">
         <f t="shared" si="1"/>
         <v>183920</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="16">
         <f t="shared" si="1"/>
         <v>298369</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="16">
         <f t="shared" si="1"/>
         <v>333739</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="16">
         <f t="shared" si="1"/>
         <v>631006</v>
       </c>
-      <c r="I29" s="18">
+      <c r="I29" s="16">
         <f t="shared" si="1"/>
         <v>700263</v>
       </c>
-      <c r="J29" s="18">
+      <c r="J29" s="16">
         <f t="shared" si="1"/>
         <v>545420</v>
       </c>
-      <c r="K29" s="18">
+      <c r="K29" s="16">
         <f t="shared" si="1"/>
         <v>1165156</v>
       </c>
@@ -4047,35 +4022,35 @@
       <c r="C30" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="16">
         <f t="shared" si="1"/>
         <v>1248617</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="16">
         <f t="shared" si="1"/>
         <v>1631860</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="16">
         <f t="shared" si="1"/>
         <v>1777653</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="16">
         <f t="shared" si="1"/>
         <v>1145510</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="16">
         <f t="shared" si="1"/>
         <v>1535684</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="16">
         <f t="shared" si="1"/>
         <v>1867982</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="16">
         <f t="shared" si="1"/>
         <v>1893893</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K30" s="16">
         <f t="shared" si="1"/>
         <v>1974713</v>
       </c>
@@ -4090,35 +4065,35 @@
       <c r="C31" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="16">
         <f t="shared" si="1"/>
         <v>393757</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="16">
         <f t="shared" si="1"/>
         <v>526048</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="16">
         <f t="shared" si="1"/>
         <v>197325</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="16">
         <f t="shared" si="1"/>
         <v>207426</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H31" s="16">
         <f t="shared" si="1"/>
         <v>267857</v>
       </c>
-      <c r="I31" s="18">
+      <c r="I31" s="16">
         <f t="shared" si="1"/>
         <v>321714</v>
       </c>
-      <c r="J31" s="18">
+      <c r="J31" s="16">
         <f t="shared" si="1"/>
         <v>234902</v>
       </c>
-      <c r="K31" s="18">
+      <c r="K31" s="16">
         <f t="shared" si="1"/>
         <v>381778</v>
       </c>
@@ -4134,39 +4109,39 @@
       <c r="C32" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="16">
         <f>SUMIF($C$6:$C$26,$C32,D$6:D$26)</f>
         <v>294470</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="16">
         <f t="shared" ref="E32:K47" si="2">SUMIF($C$6:$C$26,$C32,E$6:E$26)</f>
         <v>186951</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="16">
         <f t="shared" si="2"/>
         <v>367618</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="16">
         <f t="shared" si="2"/>
         <v>231313</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H32" s="16">
         <f t="shared" si="2"/>
         <v>104650</v>
       </c>
-      <c r="I32" s="18">
+      <c r="I32" s="16">
         <f t="shared" si="2"/>
         <v>194875</v>
       </c>
-      <c r="J32" s="18">
+      <c r="J32" s="16">
         <f t="shared" si="2"/>
         <v>213221</v>
       </c>
-      <c r="K32" s="18">
+      <c r="K32" s="16">
         <f t="shared" si="2"/>
         <v>193992</v>
       </c>
-      <c r="L32" s="18"/>
+      <c r="L32" s="16"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -4179,39 +4154,39 @@
       <c r="C33" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="16">
         <f t="shared" ref="D33:K50" si="4">SUMIF($C$6:$C$26,$C33,D$6:D$26)</f>
         <v>454644</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="16">
         <f t="shared" si="2"/>
         <v>373951</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="16">
         <f t="shared" si="2"/>
         <v>452918</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="16">
         <f t="shared" si="2"/>
         <v>341964</v>
       </c>
-      <c r="H33" s="18">
+      <c r="H33" s="16">
         <f t="shared" si="2"/>
         <v>383853</v>
       </c>
-      <c r="I33" s="18">
+      <c r="I33" s="16">
         <f t="shared" si="2"/>
         <v>371618</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="16">
         <f t="shared" si="2"/>
         <v>612583</v>
       </c>
-      <c r="K33" s="18">
+      <c r="K33" s="16">
         <f t="shared" si="2"/>
         <v>341273</v>
       </c>
-      <c r="L33" s="18"/>
+      <c r="L33" s="16"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -4224,35 +4199,35 @@
       <c r="C34" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34" s="16">
         <f t="shared" si="4"/>
         <v>280973</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="16">
         <f t="shared" si="2"/>
         <v>354725</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="16">
         <f t="shared" si="2"/>
         <v>100058</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="16">
         <f t="shared" si="2"/>
         <v>159938</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="16">
         <f t="shared" si="2"/>
         <v>413803</v>
       </c>
-      <c r="I34" s="18">
+      <c r="I34" s="16">
         <f t="shared" si="2"/>
         <v>367772</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="16">
         <f t="shared" si="2"/>
         <v>284116</v>
       </c>
-      <c r="K34" s="18">
+      <c r="K34" s="16">
         <f t="shared" si="2"/>
         <v>321618</v>
       </c>
@@ -4268,35 +4243,35 @@
       <c r="C35" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H35" s="18">
+      <c r="H35" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I35" s="18">
+      <c r="I35" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J35" s="18">
+      <c r="J35" s="16">
         <f t="shared" si="2"/>
         <v>123453</v>
       </c>
-      <c r="K35" s="18">
+      <c r="K35" s="16">
         <f t="shared" si="2"/>
         <v>287457</v>
       </c>
@@ -4312,35 +4287,35 @@
       <c r="C36" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="16">
         <f t="shared" si="4"/>
         <v>97664</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="16">
         <f t="shared" si="2"/>
         <v>175113</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="16">
         <f t="shared" si="2"/>
         <v>145525</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G36" s="16">
         <f t="shared" si="2"/>
         <v>115866</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H36" s="16">
         <f t="shared" si="2"/>
         <v>231794</v>
       </c>
-      <c r="I36" s="18">
+      <c r="I36" s="16">
         <f t="shared" si="2"/>
         <v>214229</v>
       </c>
-      <c r="J36" s="18">
+      <c r="J36" s="16">
         <f t="shared" si="2"/>
         <v>302197</v>
       </c>
-      <c r="K36" s="18">
+      <c r="K36" s="16">
         <f t="shared" si="2"/>
         <v>360759</v>
       </c>
@@ -4356,35 +4331,35 @@
       <c r="C37" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D37" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F37" s="16">
         <f t="shared" si="2"/>
         <v>95423</v>
       </c>
-      <c r="G37" s="18">
+      <c r="G37" s="16">
         <f t="shared" si="2"/>
         <v>127835</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H37" s="16">
         <f t="shared" si="2"/>
         <v>406324</v>
       </c>
-      <c r="I37" s="18">
+      <c r="I37" s="16">
         <f t="shared" si="2"/>
         <v>423569</v>
       </c>
-      <c r="J37" s="18">
+      <c r="J37" s="16">
         <f t="shared" si="2"/>
         <v>160758</v>
       </c>
-      <c r="K37" s="18">
+      <c r="K37" s="16">
         <f t="shared" si="2"/>
         <v>287874</v>
       </c>
@@ -4400,35 +4375,35 @@
       <c r="C38" t="s">
         <v>139</v>
       </c>
-      <c r="D38" s="18">
+      <c r="D38" s="16">
         <f t="shared" si="4"/>
         <v>96072</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="16">
         <f t="shared" si="2"/>
         <v>322071</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="16">
         <f t="shared" si="2"/>
         <v>337517</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="16">
         <f t="shared" si="2"/>
         <v>146034</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H38" s="16">
         <f t="shared" si="2"/>
         <v>364865</v>
       </c>
-      <c r="I38" s="18">
+      <c r="I38" s="16">
         <f t="shared" si="2"/>
         <v>414727</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="16">
         <f t="shared" si="2"/>
         <v>250822</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="16">
         <f t="shared" si="2"/>
         <v>423552</v>
       </c>
@@ -4444,35 +4419,35 @@
       <c r="C39" t="s">
         <v>140</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="16">
         <f t="shared" si="4"/>
         <v>261518</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="16">
         <f t="shared" si="2"/>
         <v>183920</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="16">
         <f t="shared" si="2"/>
         <v>202946</v>
       </c>
-      <c r="G39" s="18">
+      <c r="G39" s="16">
         <f t="shared" si="2"/>
         <v>205904</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="16">
         <f t="shared" si="2"/>
         <v>224682</v>
       </c>
-      <c r="I39" s="18">
+      <c r="I39" s="16">
         <f t="shared" si="2"/>
         <v>276694</v>
       </c>
-      <c r="J39" s="18">
+      <c r="J39" s="16">
         <f t="shared" si="2"/>
         <v>261209</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="16">
         <f t="shared" si="2"/>
         <v>348653</v>
       </c>
@@ -4488,35 +4463,35 @@
       <c r="C40" t="s">
         <v>141</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D40" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F40" s="18">
+      <c r="F40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G40" s="18">
+      <c r="G40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H40" s="18">
+      <c r="H40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I40" s="18">
+      <c r="I40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J40" s="18">
+      <c r="J40" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K40" s="18">
+      <c r="K40" s="16">
         <f t="shared" si="2"/>
         <v>241172</v>
       </c>
@@ -4532,35 +4507,35 @@
       <c r="C41" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D41" s="16">
         <f t="shared" si="4"/>
         <v>104533</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="16">
         <f t="shared" si="2"/>
         <v>331448</v>
       </c>
-      <c r="F41" s="18">
+      <c r="F41" s="16">
         <f t="shared" si="2"/>
         <v>197325</v>
       </c>
-      <c r="G41" s="18">
+      <c r="G41" s="16">
         <f t="shared" si="2"/>
         <v>207426</v>
       </c>
-      <c r="H41" s="18">
+      <c r="H41" s="16">
         <f t="shared" si="2"/>
         <v>267857</v>
       </c>
-      <c r="I41" s="18">
+      <c r="I41" s="16">
         <f t="shared" si="2"/>
         <v>220092</v>
       </c>
-      <c r="J41" s="18">
+      <c r="J41" s="16">
         <f t="shared" si="2"/>
         <v>114437</v>
       </c>
-      <c r="K41" s="18">
+      <c r="K41" s="16">
         <f t="shared" si="2"/>
         <v>119241</v>
       </c>
@@ -4576,35 +4551,35 @@
       <c r="C42" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="16">
         <f t="shared" si="4"/>
         <v>324209</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="16">
         <f t="shared" si="2"/>
         <v>253397</v>
       </c>
-      <c r="F42" s="18">
+      <c r="F42" s="16">
         <f t="shared" si="2"/>
         <v>298893</v>
       </c>
-      <c r="G42" s="18">
+      <c r="G42" s="16">
         <f t="shared" si="2"/>
         <v>116472</v>
       </c>
-      <c r="H42" s="18">
+      <c r="H42" s="16">
         <f t="shared" si="2"/>
         <v>209008</v>
       </c>
-      <c r="I42" s="18">
+      <c r="I42" s="16">
         <f t="shared" si="2"/>
         <v>284024</v>
       </c>
-      <c r="J42" s="18">
+      <c r="J42" s="16">
         <f t="shared" si="2"/>
         <v>295343</v>
       </c>
-      <c r="K42" s="18">
+      <c r="K42" s="16">
         <f t="shared" si="2"/>
         <v>303757</v>
       </c>
@@ -4620,35 +4595,35 @@
       <c r="C43" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="18">
+      <c r="D43" s="16">
         <f t="shared" si="4"/>
         <v>182673</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="16">
         <f t="shared" si="2"/>
         <v>338317</v>
       </c>
-      <c r="F43" s="18">
+      <c r="F43" s="16">
         <f t="shared" si="2"/>
         <v>224638</v>
       </c>
-      <c r="G43" s="18">
+      <c r="G43" s="16">
         <f t="shared" si="2"/>
         <v>199913</v>
       </c>
-      <c r="H43" s="18">
+      <c r="H43" s="16">
         <f t="shared" si="2"/>
         <v>157338</v>
       </c>
-      <c r="I43" s="18">
+      <c r="I43" s="16">
         <f t="shared" si="2"/>
         <v>438173</v>
       </c>
-      <c r="J43" s="18">
+      <c r="J43" s="16">
         <f t="shared" si="2"/>
         <v>416473</v>
       </c>
-      <c r="K43" s="18">
+      <c r="K43" s="16">
         <f t="shared" si="2"/>
         <v>242891</v>
       </c>
@@ -4664,35 +4639,35 @@
       <c r="C44" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="18">
+      <c r="D44" s="16">
         <f t="shared" si="4"/>
         <v>359697</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="16">
         <f t="shared" si="2"/>
         <v>395046</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="16">
         <f t="shared" si="2"/>
         <v>129871</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="16">
         <f t="shared" si="2"/>
         <v>112396</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H44" s="16">
         <f t="shared" si="2"/>
         <v>185351</v>
       </c>
-      <c r="I44" s="18">
+      <c r="I44" s="16">
         <f t="shared" si="2"/>
         <v>172879</v>
       </c>
-      <c r="J44" s="18">
+      <c r="J44" s="16">
         <f t="shared" si="2"/>
         <v>415627</v>
       </c>
-      <c r="K44" s="18">
+      <c r="K44" s="16">
         <f t="shared" si="2"/>
         <v>224008</v>
       </c>
@@ -4708,35 +4683,35 @@
       <c r="C45" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="16">
         <f t="shared" si="4"/>
         <v>289224</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="16">
         <f t="shared" si="2"/>
         <v>194600</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I45" s="18">
+      <c r="I45" s="16">
         <f t="shared" si="2"/>
         <v>101622</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="16">
         <f t="shared" si="2"/>
         <v>120465</v>
       </c>
-      <c r="K45" s="18">
+      <c r="K45" s="16">
         <f t="shared" si="2"/>
         <v>262537</v>
       </c>
@@ -4752,35 +4727,35 @@
       <c r="C46" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="18">
+      <c r="D46" s="16">
         <f t="shared" si="4"/>
         <v>281335</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="16">
         <f t="shared" si="2"/>
         <v>290674</v>
       </c>
-      <c r="F46" s="18">
+      <c r="F46" s="16">
         <f t="shared" si="2"/>
         <v>213416</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="16">
         <f t="shared" si="2"/>
         <v>138896</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="16">
         <f t="shared" si="2"/>
         <v>148716</v>
       </c>
-      <c r="I46" s="18">
+      <c r="I46" s="16">
         <f t="shared" si="2"/>
         <v>440788</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J46" s="16">
         <f t="shared" si="2"/>
         <v>118717</v>
       </c>
-      <c r="K46" s="18">
+      <c r="K46" s="16">
         <f t="shared" si="2"/>
         <v>295393</v>
       </c>
@@ -4796,35 +4771,35 @@
       <c r="C47" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D47" s="16">
         <f t="shared" si="4"/>
         <v>393053</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="16">
         <f t="shared" si="2"/>
         <v>155131</v>
       </c>
-      <c r="F47" s="18">
+      <c r="F47" s="16">
         <f t="shared" si="2"/>
         <v>197972</v>
       </c>
-      <c r="G47" s="18">
+      <c r="G47" s="16">
         <f t="shared" si="2"/>
         <v>347987</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="16">
         <f t="shared" si="2"/>
         <v>120062</v>
       </c>
-      <c r="I47" s="18">
+      <c r="I47" s="16">
         <f t="shared" si="2"/>
         <v>402641</v>
       </c>
-      <c r="J47" s="18">
+      <c r="J47" s="16">
         <f t="shared" si="2"/>
         <v>426099</v>
       </c>
-      <c r="K47" s="18">
+      <c r="K47" s="16">
         <f t="shared" si="2"/>
         <v>442987</v>
       </c>
@@ -4840,35 +4815,35 @@
       <c r="C48" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="18">
+      <c r="D48" s="16">
         <f t="shared" si="4"/>
         <v>119379</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48" s="16">
         <f t="shared" si="4"/>
         <v>160105</v>
       </c>
-      <c r="F48" s="18">
+      <c r="F48" s="16">
         <f t="shared" si="4"/>
         <v>219178</v>
       </c>
-      <c r="G48" s="18">
+      <c r="G48" s="16">
         <f t="shared" si="4"/>
         <v>189883</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="16">
         <f t="shared" si="4"/>
         <v>146168</v>
       </c>
-      <c r="I48" s="18">
+      <c r="I48" s="16">
         <f t="shared" si="4"/>
         <v>237376</v>
       </c>
-      <c r="J48" s="18">
+      <c r="J48" s="16">
         <f t="shared" si="4"/>
         <v>344725</v>
       </c>
-      <c r="K48" s="18">
+      <c r="K48" s="16">
         <f t="shared" si="4"/>
         <v>243717</v>
       </c>
@@ -4884,35 +4859,35 @@
       <c r="C49" t="s">
         <v>150</v>
       </c>
-      <c r="D49" s="18">
+      <c r="D49" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E49" s="18">
+      <c r="E49" s="16">
         <f t="shared" si="4"/>
         <v>101900</v>
       </c>
-      <c r="F49" s="18">
+      <c r="F49" s="16">
         <f t="shared" si="4"/>
         <v>364528</v>
       </c>
-      <c r="G49" s="18">
+      <c r="G49" s="16">
         <f t="shared" si="4"/>
         <v>211122</v>
       </c>
-      <c r="H49" s="18">
+      <c r="H49" s="16">
         <f t="shared" si="4"/>
         <v>354140</v>
       </c>
-      <c r="I49" s="18">
+      <c r="I49" s="16">
         <f t="shared" si="4"/>
         <v>193108</v>
       </c>
-      <c r="J49" s="18">
+      <c r="J49" s="16">
         <f t="shared" si="4"/>
         <v>248584</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="16">
         <f t="shared" si="4"/>
         <v>233292</v>
       </c>
@@ -4928,35 +4903,35 @@
       <c r="C50" t="s">
         <v>151</v>
       </c>
-      <c r="D50" s="18">
+      <c r="D50" s="16">
         <f t="shared" si="4"/>
         <v>128355</v>
       </c>
-      <c r="E50" s="18">
+      <c r="E50" s="16">
         <f t="shared" si="4"/>
         <v>135572</v>
       </c>
-      <c r="F50" s="18">
+      <c r="F50" s="16">
         <f t="shared" si="4"/>
         <v>173208</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="16">
         <f t="shared" si="4"/>
         <v>264144</v>
       </c>
-      <c r="H50" s="18">
+      <c r="H50" s="16">
         <f t="shared" si="4"/>
         <v>438135</v>
       </c>
-      <c r="I50" s="18">
+      <c r="I50" s="16">
         <f t="shared" si="4"/>
         <v>303683</v>
       </c>
-      <c r="J50" s="18">
+      <c r="J50" s="16">
         <f t="shared" si="4"/>
         <v>446278</v>
       </c>
-      <c r="K50" s="18">
+      <c r="K50" s="16">
         <f t="shared" si="4"/>
         <v>262490</v>
       </c>
@@ -4971,18 +4946,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5203,18 +5178,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
present the sales report data by state and to exclude all corporate information
</commit_message>
<xml_diff>
--- a/Modifying the worksheet.xlsx
+++ b/Modifying the worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9F142B-B2EB-48A1-9534-B65DAAEC535C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A023CDCC-88F9-4027-869C-BA712A793A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
   </bookViews>
@@ -18,6 +18,9 @@
     <sheet name="Financial Data" sheetId="2" r:id="rId3"/>
     <sheet name="Sales Report 2018 2019" sheetId="6" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Financial Data'!$A$1:$S$27</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -653,13 +656,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2487,7 +2490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,30 +2532,30 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2">
-        <v>125319</v>
+        <v>135816</v>
       </c>
       <c r="E2" s="2">
-        <v>65792</v>
+        <v>67388</v>
       </c>
       <c r="F2" s="2">
         <f>D2-E2</f>
-        <v>59527</v>
+        <v>68428</v>
       </c>
       <c r="G2" s="2">
-        <v>4667</v>
+        <v>5700</v>
       </c>
       <c r="H2" s="2">
         <f>F2-G2</f>
-        <v>54860</v>
+        <v>62728</v>
       </c>
       <c r="M2" s="1"/>
       <c r="O2" s="1"/>
@@ -2563,35 +2566,35 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2">
-        <v>433924</v>
+        <v>207163</v>
       </c>
       <c r="E3" s="2">
-        <v>101465</v>
+        <v>73705</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F20" si="0">D3-E3</f>
-        <v>332459</v>
+        <f>D3-E3</f>
+        <v>133458</v>
       </c>
       <c r="G3" s="2">
-        <v>5068</v>
+        <v>5599</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H20" si="1">F3-G3</f>
-        <v>327391</v>
+        <f>F3-G3</f>
+        <v>127859</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>71</v>
@@ -2600,507 +2603,511 @@
         <v>32</v>
       </c>
       <c r="D4" s="2">
-        <v>135816</v>
+        <v>432326</v>
       </c>
       <c r="E4" s="2">
-        <v>67388</v>
+        <v>79297</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>68428</v>
+        <f>D4-E4</f>
+        <v>353029</v>
       </c>
       <c r="G4" s="2">
-        <v>5700</v>
+        <v>4872</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="1"/>
-        <v>62728</v>
+        <f>F4-G4</f>
+        <v>348157</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2">
-        <v>233255</v>
+        <v>376263</v>
       </c>
       <c r="E5" s="2">
-        <v>83606</v>
+        <v>92698</v>
       </c>
       <c r="F5" s="2">
         <f>D5-E5</f>
-        <v>149649</v>
+        <v>283565</v>
       </c>
       <c r="G5" s="2">
-        <v>5089</v>
+        <v>5195</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="1"/>
-        <v>144560</v>
+        <f>F5-G5</f>
+        <v>278370</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2">
-        <v>128691</v>
+        <v>244975</v>
       </c>
       <c r="E6" s="2">
-        <v>67175</v>
+        <v>100834</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>61516</v>
+        <f>D6-E6</f>
+        <v>144141</v>
       </c>
       <c r="G6" s="2">
-        <v>4956</v>
+        <v>5153</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="1"/>
-        <v>56560</v>
+        <f>F6-G6</f>
+        <v>138988</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2">
-        <v>244913</v>
+        <v>201945</v>
       </c>
       <c r="E7" s="2">
-        <v>89974</v>
+        <v>83178</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>154939</v>
+        <f>D7-E7</f>
+        <v>118767</v>
       </c>
       <c r="G7" s="2">
-        <v>5062</v>
+        <v>4734</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="1"/>
-        <v>149877</v>
+        <f>F7-G7</f>
+        <v>114033</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2">
-        <v>392518</v>
+        <v>125319</v>
       </c>
       <c r="E8" s="2">
-        <v>82675</v>
+        <v>65792</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>309843</v>
+        <f>D8-E8</f>
+        <v>59527</v>
       </c>
       <c r="G8" s="2">
-        <v>6100</v>
+        <v>4667</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="1"/>
-        <v>303743</v>
+        <f>F8-G8</f>
+        <v>54860</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2">
-        <v>331773</v>
+        <v>233255</v>
       </c>
       <c r="E9" s="2">
-        <v>85288</v>
+        <v>83606</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>246485</v>
+        <f>D9-E9</f>
+        <v>149649</v>
       </c>
       <c r="G9" s="2">
-        <v>5795</v>
+        <v>5089</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="1"/>
-        <v>240690</v>
+        <f>F9-G9</f>
+        <v>144560</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2">
-        <v>244975</v>
+        <v>331773</v>
       </c>
       <c r="E10" s="2">
-        <v>100834</v>
+        <v>85288</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>144141</v>
+        <f>D10-E10</f>
+        <v>246485</v>
       </c>
       <c r="G10" s="2">
-        <v>5153</v>
+        <v>5795</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="1"/>
-        <v>138988</v>
+        <f>F10-G10</f>
+        <v>240690</v>
       </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="2">
-        <v>137925</v>
+        <v>407339</v>
       </c>
       <c r="E11" s="2">
-        <v>104528</v>
+        <v>88286</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>33397</v>
+        <f>D11-E11</f>
+        <v>319053</v>
       </c>
       <c r="G11" s="2">
-        <v>5673</v>
+        <v>4604</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="1"/>
-        <v>27724</v>
+        <f>F11-G11</f>
+        <v>314449</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2">
-        <v>207163</v>
+        <v>440462</v>
       </c>
       <c r="E12" s="2">
-        <v>73705</v>
+        <v>81912</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>133458</v>
+        <f>D12-E12</f>
+        <v>358550</v>
       </c>
       <c r="G12" s="2">
-        <v>5599</v>
+        <v>4842</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="1"/>
-        <v>127859</v>
+        <f>F12-G12</f>
+        <v>353708</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2">
-        <v>432326</v>
+        <v>149134</v>
       </c>
       <c r="E13" s="2">
-        <v>79297</v>
+        <v>87513</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>353029</v>
+        <f>D13-E13</f>
+        <v>61621</v>
       </c>
       <c r="G13" s="2">
-        <v>4872</v>
+        <v>5168</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="1"/>
-        <v>348157</v>
+        <f>F13-G13</f>
+        <v>56453</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2">
-        <v>177789</v>
+        <v>244913</v>
       </c>
       <c r="E14" s="2">
-        <v>103757</v>
+        <v>89974</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>74032</v>
+        <f>D14-E14</f>
+        <v>154939</v>
       </c>
       <c r="G14" s="2">
-        <v>5144</v>
+        <v>5062</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="1"/>
-        <v>68888</v>
+        <f>F14-G14</f>
+        <v>149877</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2">
-        <v>201945</v>
+        <v>137925</v>
       </c>
       <c r="E15" s="2">
-        <v>83178</v>
+        <v>104528</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>118767</v>
+        <f>D15-E15</f>
+        <v>33397</v>
       </c>
       <c r="G15" s="2">
-        <v>4734</v>
+        <v>5673</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="1"/>
-        <v>114033</v>
+        <f>F15-G15</f>
+        <v>27724</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2">
-        <v>461214</v>
+        <v>177789</v>
       </c>
       <c r="E16" s="2">
-        <v>86688</v>
+        <v>103757</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>374526</v>
+        <f>D16-E16</f>
+        <v>74032</v>
       </c>
       <c r="G16" s="2">
-        <v>6066</v>
+        <v>5144</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="1"/>
-        <v>368460</v>
+        <f>F16-G16</f>
+        <v>68888</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2">
-        <v>440462</v>
+        <v>433924</v>
       </c>
       <c r="E17" s="2">
-        <v>81912</v>
+        <v>101465</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>358550</v>
+        <f>D17-E17</f>
+        <v>332459</v>
       </c>
       <c r="G17" s="2">
-        <v>4842</v>
+        <v>5068</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="1"/>
-        <v>353708</v>
+        <f>F17-G17</f>
+        <v>327391</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2">
-        <v>407339</v>
+        <v>128691</v>
       </c>
       <c r="E18" s="2">
-        <v>88286</v>
+        <v>67175</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>319053</v>
+        <f>D18-E18</f>
+        <v>61516</v>
       </c>
       <c r="G18" s="2">
-        <v>4604</v>
+        <v>4956</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="1"/>
-        <v>314449</v>
+        <f>F18-G18</f>
+        <v>56560</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2">
-        <v>376263</v>
+        <v>392518</v>
       </c>
       <c r="E19" s="2">
-        <v>92698</v>
+        <v>82675</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>283565</v>
+        <f>D19-E19</f>
+        <v>309843</v>
       </c>
       <c r="G19" s="2">
-        <v>5195</v>
+        <v>6100</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="1"/>
-        <v>278370</v>
+        <f>F19-G19</f>
+        <v>303743</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
-        <v>149134</v>
+        <v>461214</v>
       </c>
       <c r="E20" s="2">
-        <v>87513</v>
+        <v>86688</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>61621</v>
+        <f>D20-E20</f>
+        <v>374526</v>
       </c>
       <c r="G20" s="2">
-        <v>5168</v>
+        <v>6066</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="1"/>
-        <v>56453</v>
+        <f>F20-G20</f>
+        <v>368460</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="18">
         <f>AVERAGE(D2:D20)</f>
         <v>276986.5263157895</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="18">
         <f>MAX(D2:D20)</f>
         <v>461214</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="18">
         <f>MIN(D2:D20)</f>
         <v>125319</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S27" xr:uid="{17D64E18-04DF-4C91-A84C-5EB5EC653CDA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H20">
+    <sortCondition ref="B2:B20"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="E24:F24"/>
   </mergeCells>
@@ -3158,18 +3165,18 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D4" s="17">
+      <c r="D4" s="20">
         <v>2018</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20">
         <v>2019</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
@@ -4946,21 +4953,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -5177,24 +5169,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA3212C-9EA0-4F60-9BC2-AD5EAEF2279B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5211,4 +5201,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>